<commit_message>
Zombie made, food product added, added moving functionality zombie, zombie follows player, food product disappears after it is picked up by player
</commit_message>
<xml_diff>
--- a/ProjectPlan2022SeniorProject.xlsx
+++ b/ProjectPlan2022SeniorProject.xlsx
@@ -3,9 +3,9 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25629"/>
   <workbookPr filterPrivacy="1" codeName="ThisWorkbook"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{C5DA118F-6065-4CA7-AEA8-30A0EA54A3FE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EACF294B-34E1-4CC4-B9D9-CF2C3B22F7BF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView minimized="1" xWindow="1884" yWindow="1884" windowWidth="17280" windowHeight="8880" tabRatio="426" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" tabRatio="426" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="ProjectSchedule" sheetId="11" r:id="rId1"/>
@@ -227,16 +227,16 @@
     <t>Adil</t>
   </si>
   <si>
-    <t>Task 2 : Add enemies, finish the screens, health counter, build a gun, shoot projectiles, scoreboard</t>
-  </si>
-  <si>
-    <t>Task 3 : Terrain finished, Work on Enemies, finsih  the scoreboard</t>
-  </si>
-  <si>
-    <t>Task 3: Complete One full wave, Make the game winnable or looseable, work on different levels</t>
-  </si>
-  <si>
     <t>Task 5 : Work on any bugs produced</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Task 2 : Add enemies, finish the screens, health counter, build a gun, shoot projectiles, scoreboard, food </t>
+  </si>
+  <si>
+    <t>Task 3 : Terrain finished, Work on Enemies, finsih  the scoreboar, build a timer</t>
+  </si>
+  <si>
+    <t>Task 3: Complete One full wave, Make the game winnable or looseable, work on different levels … // add projectiles if unable to add them by this snapshot</t>
   </si>
 </sst>
 </file>
@@ -908,6 +908,18 @@
     <xf numFmtId="0" fontId="0" fillId="10" borderId="2" xfId="12" applyFont="1" applyFill="1">
       <alignment horizontal="left" vertical="center" indent="2"/>
     </xf>
+    <xf numFmtId="166" fontId="0" fillId="7" borderId="4" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1" indent="1"/>
+    </xf>
+    <xf numFmtId="166" fontId="0" fillId="7" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1" indent="1"/>
+    </xf>
+    <xf numFmtId="166" fontId="0" fillId="7" borderId="5" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1" indent="1"/>
+    </xf>
+    <xf numFmtId="165" fontId="9" fillId="0" borderId="3" xfId="9">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="8">
       <alignment horizontal="right" indent="1"/>
     </xf>
@@ -915,18 +927,6 @@
       <alignment horizontal="right" indent="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1"/>
-    <xf numFmtId="166" fontId="0" fillId="7" borderId="4" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1" indent="1"/>
-    </xf>
-    <xf numFmtId="166" fontId="0" fillId="7" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1" indent="1"/>
-    </xf>
-    <xf numFmtId="166" fontId="0" fillId="7" borderId="5" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1" indent="1"/>
-    </xf>
-    <xf numFmtId="165" fontId="9" fillId="0" borderId="3" xfId="9">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
   </cellXfs>
   <cellStyles count="13">
     <cellStyle name="Comma" xfId="4" builtinId="3" customBuiltin="1"/>
@@ -1497,7 +1497,7 @@
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" showRuler="0" zoomScale="98" zoomScaleNormal="100" zoomScalePageLayoutView="70" workbookViewId="0">
       <pane ySplit="6" topLeftCell="A10" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="B11" sqref="B11"/>
+      <selection pane="bottomLeft" activeCell="B14" sqref="B14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="30" customHeight="1" x14ac:dyDescent="0.3"/>
@@ -1542,341 +1542,341 @@
       <c r="B3" s="77" t="s">
         <v>40</v>
       </c>
-      <c r="C3" s="85" t="s">
+      <c r="C3" s="89" t="s">
         <v>1</v>
       </c>
-      <c r="D3" s="86"/>
-      <c r="E3" s="91">
+      <c r="D3" s="90"/>
+      <c r="E3" s="88">
         <f ca="1">TODAY()</f>
-        <v>44836</v>
-      </c>
-      <c r="F3" s="91"/>
+        <v>44849</v>
+      </c>
+      <c r="F3" s="88"/>
     </row>
     <row r="4" spans="1:64" ht="30" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A4" s="59" t="s">
         <v>30</v>
       </c>
-      <c r="C4" s="85" t="s">
+      <c r="C4" s="89" t="s">
         <v>8</v>
       </c>
-      <c r="D4" s="86"/>
+      <c r="D4" s="90"/>
       <c r="E4" s="7">
         <v>1</v>
       </c>
-      <c r="I4" s="88">
+      <c r="I4" s="85">
         <f ca="1">I5</f>
-        <v>44837</v>
-      </c>
-      <c r="J4" s="89"/>
-      <c r="K4" s="89"/>
-      <c r="L4" s="89"/>
-      <c r="M4" s="89"/>
-      <c r="N4" s="89"/>
-      <c r="O4" s="90"/>
-      <c r="P4" s="88">
+        <v>44844</v>
+      </c>
+      <c r="J4" s="86"/>
+      <c r="K4" s="86"/>
+      <c r="L4" s="86"/>
+      <c r="M4" s="86"/>
+      <c r="N4" s="86"/>
+      <c r="O4" s="87"/>
+      <c r="P4" s="85">
         <f ca="1">P5</f>
-        <v>44844</v>
-      </c>
-      <c r="Q4" s="89"/>
-      <c r="R4" s="89"/>
-      <c r="S4" s="89"/>
-      <c r="T4" s="89"/>
-      <c r="U4" s="89"/>
-      <c r="V4" s="90"/>
-      <c r="W4" s="88">
+        <v>44851</v>
+      </c>
+      <c r="Q4" s="86"/>
+      <c r="R4" s="86"/>
+      <c r="S4" s="86"/>
+      <c r="T4" s="86"/>
+      <c r="U4" s="86"/>
+      <c r="V4" s="87"/>
+      <c r="W4" s="85">
         <f ca="1">W5</f>
-        <v>44851</v>
-      </c>
-      <c r="X4" s="89"/>
-      <c r="Y4" s="89"/>
-      <c r="Z4" s="89"/>
-      <c r="AA4" s="89"/>
-      <c r="AB4" s="89"/>
-      <c r="AC4" s="90"/>
-      <c r="AD4" s="88">
+        <v>44858</v>
+      </c>
+      <c r="X4" s="86"/>
+      <c r="Y4" s="86"/>
+      <c r="Z4" s="86"/>
+      <c r="AA4" s="86"/>
+      <c r="AB4" s="86"/>
+      <c r="AC4" s="87"/>
+      <c r="AD4" s="85">
         <f ca="1">AD5</f>
-        <v>44858</v>
-      </c>
-      <c r="AE4" s="89"/>
-      <c r="AF4" s="89"/>
-      <c r="AG4" s="89"/>
-      <c r="AH4" s="89"/>
-      <c r="AI4" s="89"/>
-      <c r="AJ4" s="90"/>
-      <c r="AK4" s="88">
+        <v>44865</v>
+      </c>
+      <c r="AE4" s="86"/>
+      <c r="AF4" s="86"/>
+      <c r="AG4" s="86"/>
+      <c r="AH4" s="86"/>
+      <c r="AI4" s="86"/>
+      <c r="AJ4" s="87"/>
+      <c r="AK4" s="85">
         <f ca="1">AK5</f>
-        <v>44865</v>
-      </c>
-      <c r="AL4" s="89"/>
-      <c r="AM4" s="89"/>
-      <c r="AN4" s="89"/>
-      <c r="AO4" s="89"/>
-      <c r="AP4" s="89"/>
-      <c r="AQ4" s="90"/>
-      <c r="AR4" s="88">
+        <v>44872</v>
+      </c>
+      <c r="AL4" s="86"/>
+      <c r="AM4" s="86"/>
+      <c r="AN4" s="86"/>
+      <c r="AO4" s="86"/>
+      <c r="AP4" s="86"/>
+      <c r="AQ4" s="87"/>
+      <c r="AR4" s="85">
         <f ca="1">AR5</f>
-        <v>44872</v>
-      </c>
-      <c r="AS4" s="89"/>
-      <c r="AT4" s="89"/>
-      <c r="AU4" s="89"/>
-      <c r="AV4" s="89"/>
-      <c r="AW4" s="89"/>
-      <c r="AX4" s="90"/>
-      <c r="AY4" s="88">
+        <v>44879</v>
+      </c>
+      <c r="AS4" s="86"/>
+      <c r="AT4" s="86"/>
+      <c r="AU4" s="86"/>
+      <c r="AV4" s="86"/>
+      <c r="AW4" s="86"/>
+      <c r="AX4" s="87"/>
+      <c r="AY4" s="85">
         <f ca="1">AY5</f>
-        <v>44879</v>
-      </c>
-      <c r="AZ4" s="89"/>
-      <c r="BA4" s="89"/>
-      <c r="BB4" s="89"/>
-      <c r="BC4" s="89"/>
-      <c r="BD4" s="89"/>
-      <c r="BE4" s="90"/>
-      <c r="BF4" s="88">
+        <v>44886</v>
+      </c>
+      <c r="AZ4" s="86"/>
+      <c r="BA4" s="86"/>
+      <c r="BB4" s="86"/>
+      <c r="BC4" s="86"/>
+      <c r="BD4" s="86"/>
+      <c r="BE4" s="87"/>
+      <c r="BF4" s="85">
         <f ca="1">BF5</f>
-        <v>44886</v>
-      </c>
-      <c r="BG4" s="89"/>
-      <c r="BH4" s="89"/>
-      <c r="BI4" s="89"/>
-      <c r="BJ4" s="89"/>
-      <c r="BK4" s="89"/>
-      <c r="BL4" s="90"/>
+        <v>44893</v>
+      </c>
+      <c r="BG4" s="86"/>
+      <c r="BH4" s="86"/>
+      <c r="BI4" s="86"/>
+      <c r="BJ4" s="86"/>
+      <c r="BK4" s="86"/>
+      <c r="BL4" s="87"/>
     </row>
     <row r="5" spans="1:64" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A5" s="59" t="s">
         <v>31</v>
       </c>
-      <c r="B5" s="87"/>
-      <c r="C5" s="87"/>
-      <c r="D5" s="87"/>
-      <c r="E5" s="87"/>
-      <c r="F5" s="87"/>
-      <c r="G5" s="87"/>
+      <c r="B5" s="91"/>
+      <c r="C5" s="91"/>
+      <c r="D5" s="91"/>
+      <c r="E5" s="91"/>
+      <c r="F5" s="91"/>
+      <c r="G5" s="91"/>
       <c r="I5" s="11">
         <f ca="1">Project_Start-WEEKDAY(Project_Start,1)+2+7*(Display_Week-1)</f>
-        <v>44837</v>
+        <v>44844</v>
       </c>
       <c r="J5" s="10">
         <f ca="1">I5+1</f>
-        <v>44838</v>
+        <v>44845</v>
       </c>
       <c r="K5" s="10">
         <f t="shared" ref="K5:AX5" ca="1" si="0">J5+1</f>
-        <v>44839</v>
+        <v>44846</v>
       </c>
       <c r="L5" s="10">
         <f t="shared" ca="1" si="0"/>
-        <v>44840</v>
+        <v>44847</v>
       </c>
       <c r="M5" s="10">
         <f t="shared" ca="1" si="0"/>
-        <v>44841</v>
+        <v>44848</v>
       </c>
       <c r="N5" s="10">
         <f t="shared" ca="1" si="0"/>
-        <v>44842</v>
+        <v>44849</v>
       </c>
       <c r="O5" s="12">
         <f t="shared" ca="1" si="0"/>
-        <v>44843</v>
+        <v>44850</v>
       </c>
       <c r="P5" s="11">
         <f ca="1">O5+1</f>
-        <v>44844</v>
+        <v>44851</v>
       </c>
       <c r="Q5" s="10">
         <f ca="1">P5+1</f>
-        <v>44845</v>
+        <v>44852</v>
       </c>
       <c r="R5" s="10">
         <f t="shared" ca="1" si="0"/>
-        <v>44846</v>
+        <v>44853</v>
       </c>
       <c r="S5" s="10">
         <f t="shared" ca="1" si="0"/>
-        <v>44847</v>
+        <v>44854</v>
       </c>
       <c r="T5" s="10">
         <f t="shared" ca="1" si="0"/>
-        <v>44848</v>
+        <v>44855</v>
       </c>
       <c r="U5" s="10">
         <f t="shared" ca="1" si="0"/>
-        <v>44849</v>
+        <v>44856</v>
       </c>
       <c r="V5" s="12">
         <f t="shared" ca="1" si="0"/>
-        <v>44850</v>
+        <v>44857</v>
       </c>
       <c r="W5" s="11">
         <f ca="1">V5+1</f>
-        <v>44851</v>
+        <v>44858</v>
       </c>
       <c r="X5" s="10">
         <f ca="1">W5+1</f>
-        <v>44852</v>
+        <v>44859</v>
       </c>
       <c r="Y5" s="10">
         <f t="shared" ca="1" si="0"/>
-        <v>44853</v>
+        <v>44860</v>
       </c>
       <c r="Z5" s="10">
         <f t="shared" ca="1" si="0"/>
-        <v>44854</v>
+        <v>44861</v>
       </c>
       <c r="AA5" s="10">
         <f t="shared" ca="1" si="0"/>
-        <v>44855</v>
+        <v>44862</v>
       </c>
       <c r="AB5" s="10">
         <f t="shared" ca="1" si="0"/>
-        <v>44856</v>
+        <v>44863</v>
       </c>
       <c r="AC5" s="12">
         <f t="shared" ca="1" si="0"/>
-        <v>44857</v>
+        <v>44864</v>
       </c>
       <c r="AD5" s="11">
         <f ca="1">AC5+1</f>
-        <v>44858</v>
+        <v>44865</v>
       </c>
       <c r="AE5" s="10">
         <f ca="1">AD5+1</f>
-        <v>44859</v>
+        <v>44866</v>
       </c>
       <c r="AF5" s="10">
         <f t="shared" ca="1" si="0"/>
-        <v>44860</v>
+        <v>44867</v>
       </c>
       <c r="AG5" s="10">
         <f t="shared" ca="1" si="0"/>
-        <v>44861</v>
+        <v>44868</v>
       </c>
       <c r="AH5" s="10">
         <f t="shared" ca="1" si="0"/>
-        <v>44862</v>
+        <v>44869</v>
       </c>
       <c r="AI5" s="10">
         <f t="shared" ca="1" si="0"/>
-        <v>44863</v>
+        <v>44870</v>
       </c>
       <c r="AJ5" s="12">
         <f t="shared" ca="1" si="0"/>
-        <v>44864</v>
+        <v>44871</v>
       </c>
       <c r="AK5" s="11">
         <f ca="1">AJ5+1</f>
-        <v>44865</v>
+        <v>44872</v>
       </c>
       <c r="AL5" s="10">
         <f ca="1">AK5+1</f>
-        <v>44866</v>
+        <v>44873</v>
       </c>
       <c r="AM5" s="10">
         <f t="shared" ca="1" si="0"/>
-        <v>44867</v>
+        <v>44874</v>
       </c>
       <c r="AN5" s="10">
         <f t="shared" ca="1" si="0"/>
-        <v>44868</v>
+        <v>44875</v>
       </c>
       <c r="AO5" s="10">
         <f t="shared" ca="1" si="0"/>
-        <v>44869</v>
+        <v>44876</v>
       </c>
       <c r="AP5" s="10">
         <f t="shared" ca="1" si="0"/>
-        <v>44870</v>
+        <v>44877</v>
       </c>
       <c r="AQ5" s="12">
         <f t="shared" ca="1" si="0"/>
-        <v>44871</v>
+        <v>44878</v>
       </c>
       <c r="AR5" s="11">
         <f ca="1">AQ5+1</f>
-        <v>44872</v>
+        <v>44879</v>
       </c>
       <c r="AS5" s="10">
         <f ca="1">AR5+1</f>
-        <v>44873</v>
+        <v>44880</v>
       </c>
       <c r="AT5" s="10">
         <f t="shared" ca="1" si="0"/>
-        <v>44874</v>
+        <v>44881</v>
       </c>
       <c r="AU5" s="10">
         <f t="shared" ca="1" si="0"/>
-        <v>44875</v>
+        <v>44882</v>
       </c>
       <c r="AV5" s="10">
         <f t="shared" ca="1" si="0"/>
-        <v>44876</v>
+        <v>44883</v>
       </c>
       <c r="AW5" s="10">
         <f t="shared" ca="1" si="0"/>
-        <v>44877</v>
+        <v>44884</v>
       </c>
       <c r="AX5" s="12">
         <f t="shared" ca="1" si="0"/>
-        <v>44878</v>
+        <v>44885</v>
       </c>
       <c r="AY5" s="11">
         <f ca="1">AX5+1</f>
-        <v>44879</v>
+        <v>44886</v>
       </c>
       <c r="AZ5" s="10">
         <f ca="1">AY5+1</f>
-        <v>44880</v>
+        <v>44887</v>
       </c>
       <c r="BA5" s="10">
         <f t="shared" ref="BA5:BE5" ca="1" si="1">AZ5+1</f>
-        <v>44881</v>
+        <v>44888</v>
       </c>
       <c r="BB5" s="10">
         <f t="shared" ca="1" si="1"/>
-        <v>44882</v>
+        <v>44889</v>
       </c>
       <c r="BC5" s="10">
         <f t="shared" ca="1" si="1"/>
-        <v>44883</v>
+        <v>44890</v>
       </c>
       <c r="BD5" s="10">
         <f t="shared" ca="1" si="1"/>
-        <v>44884</v>
+        <v>44891</v>
       </c>
       <c r="BE5" s="12">
         <f t="shared" ca="1" si="1"/>
-        <v>44885</v>
+        <v>44892</v>
       </c>
       <c r="BF5" s="11">
         <f ca="1">BE5+1</f>
-        <v>44886</v>
+        <v>44893</v>
       </c>
       <c r="BG5" s="10">
         <f ca="1">BF5+1</f>
-        <v>44887</v>
+        <v>44894</v>
       </c>
       <c r="BH5" s="10">
         <f t="shared" ref="BH5:BL5" ca="1" si="2">BG5+1</f>
-        <v>44888</v>
+        <v>44895</v>
       </c>
       <c r="BI5" s="10">
         <f t="shared" ca="1" si="2"/>
-        <v>44889</v>
+        <v>44896</v>
       </c>
       <c r="BJ5" s="10">
         <f t="shared" ca="1" si="2"/>
-        <v>44890</v>
+        <v>44897</v>
       </c>
       <c r="BK5" s="10">
         <f t="shared" ca="1" si="2"/>
-        <v>44891</v>
+        <v>44898</v>
       </c>
       <c r="BL5" s="12">
         <f t="shared" ca="1" si="2"/>
-        <v>44892</v>
+        <v>44899</v>
       </c>
     </row>
     <row r="6" spans="1:64" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
@@ -2426,7 +2426,7 @@
     <row r="11" spans="1:64" s="3" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A11" s="59"/>
       <c r="B11" s="81" t="s">
-        <v>50</v>
+        <v>51</v>
       </c>
       <c r="C11" s="82" t="s">
         <v>48</v>
@@ -2505,7 +2505,7 @@
     <row r="12" spans="1:64" s="3" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A12" s="58"/>
       <c r="B12" s="81" t="s">
-        <v>51</v>
+        <v>52</v>
       </c>
       <c r="C12" s="82" t="s">
         <v>49</v>
@@ -2657,7 +2657,7 @@
     <row r="14" spans="1:64" s="3" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A14" s="58"/>
       <c r="B14" s="83" t="s">
-        <v>52</v>
+        <v>53</v>
       </c>
       <c r="C14" s="72" t="s">
         <v>46</v>
@@ -2809,7 +2809,7 @@
     <row r="16" spans="1:64" s="3" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A16" s="58"/>
       <c r="B16" s="84" t="s">
-        <v>53</v>
+        <v>50</v>
       </c>
       <c r="C16" s="74"/>
       <c r="D16" s="37">
@@ -3119,6 +3119,11 @@
     </row>
   </sheetData>
   <mergeCells count="12">
+    <mergeCell ref="C3:D3"/>
+    <mergeCell ref="C4:D4"/>
+    <mergeCell ref="B5:G5"/>
+    <mergeCell ref="AK4:AQ4"/>
+    <mergeCell ref="AR4:AX4"/>
     <mergeCell ref="AY4:BE4"/>
     <mergeCell ref="BF4:BL4"/>
     <mergeCell ref="E3:F3"/>
@@ -3126,11 +3131,6 @@
     <mergeCell ref="P4:V4"/>
     <mergeCell ref="W4:AC4"/>
     <mergeCell ref="AD4:AJ4"/>
-    <mergeCell ref="C3:D3"/>
-    <mergeCell ref="C4:D4"/>
-    <mergeCell ref="B5:G5"/>
-    <mergeCell ref="AK4:AQ4"/>
-    <mergeCell ref="AR4:AX4"/>
   </mergeCells>
   <conditionalFormatting sqref="D7:D19">
     <cfRule type="dataBar" priority="18">

</xml_diff>

<commit_message>
read me snapshot-2 added
</commit_message>
<xml_diff>
--- a/ProjectPlan2022SeniorProject.xlsx
+++ b/ProjectPlan2022SeniorProject.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25629"/>
   <workbookPr filterPrivacy="1" codeName="ThisWorkbook"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9538FC59-69DC-4C90-B01A-BE008168AB47}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0D1E181B-1B9D-4D9A-B028-1F1EA388DAB0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" tabRatio="426" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -1496,7 +1496,7 @@
   <dimension ref="A1:BL22"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" showRuler="0" zoomScale="98" zoomScaleNormal="100" zoomScalePageLayoutView="70" workbookViewId="0">
-      <pane ySplit="6" topLeftCell="A8" activePane="bottomLeft" state="frozen"/>
+      <pane ySplit="6" topLeftCell="A12" activePane="bottomLeft" state="frozen"/>
       <selection pane="bottomLeft" activeCell="B9" sqref="B9"/>
     </sheetView>
   </sheetViews>

</xml_diff>

<commit_message>
Enemy Spawns randomly on level 1
</commit_message>
<xml_diff>
--- a/ProjectPlan2022SeniorProject.xlsx
+++ b/ProjectPlan2022SeniorProject.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25726"/>
   <workbookPr filterPrivacy="1" codeName="ThisWorkbook"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B315E1E5-2B9F-4450-8237-BF52E6C5F17F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{51DB5F2A-DE3B-48C2-98DC-8ACA78CE50BF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" tabRatio="426" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -908,6 +908,13 @@
     <xf numFmtId="0" fontId="0" fillId="10" borderId="2" xfId="12" applyFont="1" applyFill="1">
       <alignment horizontal="left" vertical="center" indent="2"/>
     </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="8">
+      <alignment horizontal="right" indent="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="7" xfId="8" applyBorder="1">
+      <alignment horizontal="right" indent="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1"/>
     <xf numFmtId="166" fontId="0" fillId="7" borderId="4" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1" indent="1"/>
     </xf>
@@ -920,13 +927,6 @@
     <xf numFmtId="165" fontId="9" fillId="0" borderId="3" xfId="9">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="8">
-      <alignment horizontal="right" indent="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="7" xfId="8" applyBorder="1">
-      <alignment horizontal="right" indent="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="13">
     <cellStyle name="Comma" xfId="4" builtinId="3" customBuiltin="1"/>
@@ -1496,7 +1496,7 @@
   <dimension ref="A1:BL22"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" showRuler="0" zoomScale="98" zoomScaleNormal="100" zoomScalePageLayoutView="70" workbookViewId="0">
-      <pane ySplit="6" topLeftCell="A11" activePane="bottomLeft" state="frozen"/>
+      <pane ySplit="6" topLeftCell="A12" activePane="bottomLeft" state="frozen"/>
       <selection pane="bottomLeft" activeCell="F14" sqref="F14"/>
     </sheetView>
   </sheetViews>
@@ -1542,118 +1542,118 @@
       <c r="B3" s="77" t="s">
         <v>40</v>
       </c>
-      <c r="C3" s="89" t="s">
+      <c r="C3" s="85" t="s">
         <v>1</v>
       </c>
-      <c r="D3" s="90"/>
-      <c r="E3" s="88">
+      <c r="D3" s="86"/>
+      <c r="E3" s="91">
         <f ca="1">TODAY()</f>
         <v>44871</v>
       </c>
-      <c r="F3" s="88"/>
+      <c r="F3" s="91"/>
     </row>
     <row r="4" spans="1:64" ht="30" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A4" s="59" t="s">
         <v>30</v>
       </c>
-      <c r="C4" s="89" t="s">
+      <c r="C4" s="85" t="s">
         <v>8</v>
       </c>
-      <c r="D4" s="90"/>
+      <c r="D4" s="86"/>
       <c r="E4" s="7">
         <v>1</v>
       </c>
-      <c r="I4" s="85">
+      <c r="I4" s="88">
         <f ca="1">I5</f>
         <v>44872</v>
       </c>
-      <c r="J4" s="86"/>
-      <c r="K4" s="86"/>
-      <c r="L4" s="86"/>
-      <c r="M4" s="86"/>
-      <c r="N4" s="86"/>
-      <c r="O4" s="87"/>
-      <c r="P4" s="85">
+      <c r="J4" s="89"/>
+      <c r="K4" s="89"/>
+      <c r="L4" s="89"/>
+      <c r="M4" s="89"/>
+      <c r="N4" s="89"/>
+      <c r="O4" s="90"/>
+      <c r="P4" s="88">
         <f ca="1">P5</f>
         <v>44879</v>
       </c>
-      <c r="Q4" s="86"/>
-      <c r="R4" s="86"/>
-      <c r="S4" s="86"/>
-      <c r="T4" s="86"/>
-      <c r="U4" s="86"/>
-      <c r="V4" s="87"/>
-      <c r="W4" s="85">
+      <c r="Q4" s="89"/>
+      <c r="R4" s="89"/>
+      <c r="S4" s="89"/>
+      <c r="T4" s="89"/>
+      <c r="U4" s="89"/>
+      <c r="V4" s="90"/>
+      <c r="W4" s="88">
         <f ca="1">W5</f>
         <v>44886</v>
       </c>
-      <c r="X4" s="86"/>
-      <c r="Y4" s="86"/>
-      <c r="Z4" s="86"/>
-      <c r="AA4" s="86"/>
-      <c r="AB4" s="86"/>
-      <c r="AC4" s="87"/>
-      <c r="AD4" s="85">
+      <c r="X4" s="89"/>
+      <c r="Y4" s="89"/>
+      <c r="Z4" s="89"/>
+      <c r="AA4" s="89"/>
+      <c r="AB4" s="89"/>
+      <c r="AC4" s="90"/>
+      <c r="AD4" s="88">
         <f ca="1">AD5</f>
         <v>44893</v>
       </c>
-      <c r="AE4" s="86"/>
-      <c r="AF4" s="86"/>
-      <c r="AG4" s="86"/>
-      <c r="AH4" s="86"/>
-      <c r="AI4" s="86"/>
-      <c r="AJ4" s="87"/>
-      <c r="AK4" s="85">
+      <c r="AE4" s="89"/>
+      <c r="AF4" s="89"/>
+      <c r="AG4" s="89"/>
+      <c r="AH4" s="89"/>
+      <c r="AI4" s="89"/>
+      <c r="AJ4" s="90"/>
+      <c r="AK4" s="88">
         <f ca="1">AK5</f>
         <v>44900</v>
       </c>
-      <c r="AL4" s="86"/>
-      <c r="AM4" s="86"/>
-      <c r="AN4" s="86"/>
-      <c r="AO4" s="86"/>
-      <c r="AP4" s="86"/>
-      <c r="AQ4" s="87"/>
-      <c r="AR4" s="85">
+      <c r="AL4" s="89"/>
+      <c r="AM4" s="89"/>
+      <c r="AN4" s="89"/>
+      <c r="AO4" s="89"/>
+      <c r="AP4" s="89"/>
+      <c r="AQ4" s="90"/>
+      <c r="AR4" s="88">
         <f ca="1">AR5</f>
         <v>44907</v>
       </c>
-      <c r="AS4" s="86"/>
-      <c r="AT4" s="86"/>
-      <c r="AU4" s="86"/>
-      <c r="AV4" s="86"/>
-      <c r="AW4" s="86"/>
-      <c r="AX4" s="87"/>
-      <c r="AY4" s="85">
+      <c r="AS4" s="89"/>
+      <c r="AT4" s="89"/>
+      <c r="AU4" s="89"/>
+      <c r="AV4" s="89"/>
+      <c r="AW4" s="89"/>
+      <c r="AX4" s="90"/>
+      <c r="AY4" s="88">
         <f ca="1">AY5</f>
         <v>44914</v>
       </c>
-      <c r="AZ4" s="86"/>
-      <c r="BA4" s="86"/>
-      <c r="BB4" s="86"/>
-      <c r="BC4" s="86"/>
-      <c r="BD4" s="86"/>
-      <c r="BE4" s="87"/>
-      <c r="BF4" s="85">
+      <c r="AZ4" s="89"/>
+      <c r="BA4" s="89"/>
+      <c r="BB4" s="89"/>
+      <c r="BC4" s="89"/>
+      <c r="BD4" s="89"/>
+      <c r="BE4" s="90"/>
+      <c r="BF4" s="88">
         <f ca="1">BF5</f>
         <v>44921</v>
       </c>
-      <c r="BG4" s="86"/>
-      <c r="BH4" s="86"/>
-      <c r="BI4" s="86"/>
-      <c r="BJ4" s="86"/>
-      <c r="BK4" s="86"/>
-      <c r="BL4" s="87"/>
+      <c r="BG4" s="89"/>
+      <c r="BH4" s="89"/>
+      <c r="BI4" s="89"/>
+      <c r="BJ4" s="89"/>
+      <c r="BK4" s="89"/>
+      <c r="BL4" s="90"/>
     </row>
     <row r="5" spans="1:64" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A5" s="59" t="s">
         <v>31</v>
       </c>
-      <c r="B5" s="91"/>
-      <c r="C5" s="91"/>
-      <c r="D5" s="91"/>
-      <c r="E5" s="91"/>
-      <c r="F5" s="91"/>
-      <c r="G5" s="91"/>
+      <c r="B5" s="87"/>
+      <c r="C5" s="87"/>
+      <c r="D5" s="87"/>
+      <c r="E5" s="87"/>
+      <c r="F5" s="87"/>
+      <c r="G5" s="87"/>
       <c r="I5" s="11">
         <f ca="1">Project_Start-WEEKDAY(Project_Start,1)+2+7*(Display_Week-1)</f>
         <v>44872</v>
@@ -3119,11 +3119,6 @@
     </row>
   </sheetData>
   <mergeCells count="12">
-    <mergeCell ref="C3:D3"/>
-    <mergeCell ref="C4:D4"/>
-    <mergeCell ref="B5:G5"/>
-    <mergeCell ref="AK4:AQ4"/>
-    <mergeCell ref="AR4:AX4"/>
     <mergeCell ref="AY4:BE4"/>
     <mergeCell ref="BF4:BL4"/>
     <mergeCell ref="E3:F3"/>
@@ -3131,6 +3126,11 @@
     <mergeCell ref="P4:V4"/>
     <mergeCell ref="W4:AC4"/>
     <mergeCell ref="AD4:AJ4"/>
+    <mergeCell ref="C3:D3"/>
+    <mergeCell ref="C4:D4"/>
+    <mergeCell ref="B5:G5"/>
+    <mergeCell ref="AK4:AQ4"/>
+    <mergeCell ref="AR4:AX4"/>
   </mergeCells>
   <conditionalFormatting sqref="D7:D19">
     <cfRule type="dataBar" priority="18">

</xml_diff>

<commit_message>
Updated project plan and added read me page
</commit_message>
<xml_diff>
--- a/ProjectPlan2022SeniorProject.xlsx
+++ b/ProjectPlan2022SeniorProject.xlsx
@@ -1,9 +1,9 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25726"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25831"/>
   <workbookPr filterPrivacy="1" codeName="ThisWorkbook"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{90ED586A-C986-4062-B415-9F06571A4439}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D5486462-DB59-44E0-B228-E9475AC20CFC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" tabRatio="426" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -41,7 +41,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="56" uniqueCount="54">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="57" uniqueCount="55">
   <si>
     <t>Insert new rows ABOVE this one</t>
   </si>
@@ -191,9 +191,6 @@
     <t>Phase 4- Troubleshooting and Debugging</t>
   </si>
   <si>
-    <t>All</t>
-  </si>
-  <si>
     <t>Project Name</t>
   </si>
   <si>
@@ -237,6 +234,12 @@
   </si>
   <si>
     <t>Task 5 : only guns, enemy attack and level transitions left</t>
+  </si>
+  <si>
+    <t xml:space="preserve">All Done Game finished at our best </t>
+  </si>
+  <si>
+    <t>Done with final project</t>
   </si>
 </sst>
 </file>
@@ -908,6 +911,13 @@
     <xf numFmtId="0" fontId="0" fillId="10" borderId="2" xfId="12" applyFont="1" applyFill="1">
       <alignment horizontal="left" vertical="center" indent="2"/>
     </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="8">
+      <alignment horizontal="right" indent="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="7" xfId="8" applyBorder="1">
+      <alignment horizontal="right" indent="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1"/>
     <xf numFmtId="166" fontId="0" fillId="7" borderId="4" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1" indent="1"/>
     </xf>
@@ -920,13 +930,6 @@
     <xf numFmtId="165" fontId="9" fillId="0" borderId="3" xfId="9">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="8">
-      <alignment horizontal="right" indent="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="7" xfId="8" applyBorder="1">
-      <alignment horizontal="right" indent="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="13">
     <cellStyle name="Comma" xfId="4" builtinId="3" customBuiltin="1"/>
@@ -1496,8 +1499,8 @@
   <dimension ref="A1:BL22"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" showRuler="0" zoomScale="98" zoomScaleNormal="100" zoomScalePageLayoutView="70" workbookViewId="0">
-      <pane ySplit="6" topLeftCell="A12" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="D16" sqref="D16"/>
+      <pane ySplit="6" topLeftCell="A13" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="Q17" sqref="Q17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="30" customHeight="1" x14ac:dyDescent="0.3"/>
@@ -1517,7 +1520,7 @@
     <row r="1" spans="1:64" ht="30" customHeight="1" x14ac:dyDescent="0.5">
       <c r="A1" s="59"/>
       <c r="B1" s="79" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="C1" s="1"/>
       <c r="D1" s="2"/>
@@ -1540,343 +1543,343 @@
         <v>29</v>
       </c>
       <c r="B3" s="77" t="s">
-        <v>40</v>
-      </c>
-      <c r="C3" s="89" t="s">
+        <v>39</v>
+      </c>
+      <c r="C3" s="85" t="s">
         <v>1</v>
       </c>
-      <c r="D3" s="90"/>
-      <c r="E3" s="88">
+      <c r="D3" s="86"/>
+      <c r="E3" s="91">
         <f ca="1">TODAY()</f>
-        <v>44892</v>
-      </c>
-      <c r="F3" s="88"/>
+        <v>44909</v>
+      </c>
+      <c r="F3" s="91"/>
     </row>
     <row r="4" spans="1:64" ht="30" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A4" s="59" t="s">
         <v>30</v>
       </c>
-      <c r="C4" s="89" t="s">
+      <c r="C4" s="85" t="s">
         <v>8</v>
       </c>
-      <c r="D4" s="90"/>
+      <c r="D4" s="86"/>
       <c r="E4" s="7">
         <v>1</v>
       </c>
-      <c r="I4" s="85">
+      <c r="I4" s="88">
         <f ca="1">I5</f>
-        <v>44893</v>
-      </c>
-      <c r="J4" s="86"/>
-      <c r="K4" s="86"/>
-      <c r="L4" s="86"/>
-      <c r="M4" s="86"/>
-      <c r="N4" s="86"/>
-      <c r="O4" s="87"/>
-      <c r="P4" s="85">
+        <v>44907</v>
+      </c>
+      <c r="J4" s="89"/>
+      <c r="K4" s="89"/>
+      <c r="L4" s="89"/>
+      <c r="M4" s="89"/>
+      <c r="N4" s="89"/>
+      <c r="O4" s="90"/>
+      <c r="P4" s="88">
         <f ca="1">P5</f>
-        <v>44900</v>
-      </c>
-      <c r="Q4" s="86"/>
-      <c r="R4" s="86"/>
-      <c r="S4" s="86"/>
-      <c r="T4" s="86"/>
-      <c r="U4" s="86"/>
-      <c r="V4" s="87"/>
-      <c r="W4" s="85">
+        <v>44914</v>
+      </c>
+      <c r="Q4" s="89"/>
+      <c r="R4" s="89"/>
+      <c r="S4" s="89"/>
+      <c r="T4" s="89"/>
+      <c r="U4" s="89"/>
+      <c r="V4" s="90"/>
+      <c r="W4" s="88">
         <f ca="1">W5</f>
-        <v>44907</v>
-      </c>
-      <c r="X4" s="86"/>
-      <c r="Y4" s="86"/>
-      <c r="Z4" s="86"/>
-      <c r="AA4" s="86"/>
-      <c r="AB4" s="86"/>
-      <c r="AC4" s="87"/>
-      <c r="AD4" s="85">
+        <v>44921</v>
+      </c>
+      <c r="X4" s="89"/>
+      <c r="Y4" s="89"/>
+      <c r="Z4" s="89"/>
+      <c r="AA4" s="89"/>
+      <c r="AB4" s="89"/>
+      <c r="AC4" s="90"/>
+      <c r="AD4" s="88">
         <f ca="1">AD5</f>
-        <v>44914</v>
-      </c>
-      <c r="AE4" s="86"/>
-      <c r="AF4" s="86"/>
-      <c r="AG4" s="86"/>
-      <c r="AH4" s="86"/>
-      <c r="AI4" s="86"/>
-      <c r="AJ4" s="87"/>
-      <c r="AK4" s="85">
+        <v>44928</v>
+      </c>
+      <c r="AE4" s="89"/>
+      <c r="AF4" s="89"/>
+      <c r="AG4" s="89"/>
+      <c r="AH4" s="89"/>
+      <c r="AI4" s="89"/>
+      <c r="AJ4" s="90"/>
+      <c r="AK4" s="88">
         <f ca="1">AK5</f>
-        <v>44921</v>
-      </c>
-      <c r="AL4" s="86"/>
-      <c r="AM4" s="86"/>
-      <c r="AN4" s="86"/>
-      <c r="AO4" s="86"/>
-      <c r="AP4" s="86"/>
-      <c r="AQ4" s="87"/>
-      <c r="AR4" s="85">
+        <v>44935</v>
+      </c>
+      <c r="AL4" s="89"/>
+      <c r="AM4" s="89"/>
+      <c r="AN4" s="89"/>
+      <c r="AO4" s="89"/>
+      <c r="AP4" s="89"/>
+      <c r="AQ4" s="90"/>
+      <c r="AR4" s="88">
         <f ca="1">AR5</f>
-        <v>44928</v>
-      </c>
-      <c r="AS4" s="86"/>
-      <c r="AT4" s="86"/>
-      <c r="AU4" s="86"/>
-      <c r="AV4" s="86"/>
-      <c r="AW4" s="86"/>
-      <c r="AX4" s="87"/>
-      <c r="AY4" s="85">
+        <v>44942</v>
+      </c>
+      <c r="AS4" s="89"/>
+      <c r="AT4" s="89"/>
+      <c r="AU4" s="89"/>
+      <c r="AV4" s="89"/>
+      <c r="AW4" s="89"/>
+      <c r="AX4" s="90"/>
+      <c r="AY4" s="88">
         <f ca="1">AY5</f>
-        <v>44935</v>
-      </c>
-      <c r="AZ4" s="86"/>
-      <c r="BA4" s="86"/>
-      <c r="BB4" s="86"/>
-      <c r="BC4" s="86"/>
-      <c r="BD4" s="86"/>
-      <c r="BE4" s="87"/>
-      <c r="BF4" s="85">
+        <v>44949</v>
+      </c>
+      <c r="AZ4" s="89"/>
+      <c r="BA4" s="89"/>
+      <c r="BB4" s="89"/>
+      <c r="BC4" s="89"/>
+      <c r="BD4" s="89"/>
+      <c r="BE4" s="90"/>
+      <c r="BF4" s="88">
         <f ca="1">BF5</f>
-        <v>44942</v>
-      </c>
-      <c r="BG4" s="86"/>
-      <c r="BH4" s="86"/>
-      <c r="BI4" s="86"/>
-      <c r="BJ4" s="86"/>
-      <c r="BK4" s="86"/>
-      <c r="BL4" s="87"/>
+        <v>44956</v>
+      </c>
+      <c r="BG4" s="89"/>
+      <c r="BH4" s="89"/>
+      <c r="BI4" s="89"/>
+      <c r="BJ4" s="89"/>
+      <c r="BK4" s="89"/>
+      <c r="BL4" s="90"/>
     </row>
     <row r="5" spans="1:64" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A5" s="59" t="s">
         <v>31</v>
       </c>
-      <c r="B5" s="91"/>
-      <c r="C5" s="91"/>
-      <c r="D5" s="91"/>
-      <c r="E5" s="91"/>
-      <c r="F5" s="91"/>
-      <c r="G5" s="91"/>
+      <c r="B5" s="87"/>
+      <c r="C5" s="87"/>
+      <c r="D5" s="87"/>
+      <c r="E5" s="87"/>
+      <c r="F5" s="87"/>
+      <c r="G5" s="87"/>
       <c r="I5" s="11">
         <f ca="1">Project_Start-WEEKDAY(Project_Start,1)+2+7*(Display_Week-1)</f>
-        <v>44893</v>
+        <v>44907</v>
       </c>
       <c r="J5" s="10">
         <f ca="1">I5+1</f>
-        <v>44894</v>
+        <v>44908</v>
       </c>
       <c r="K5" s="10">
         <f t="shared" ref="K5:AX5" ca="1" si="0">J5+1</f>
-        <v>44895</v>
+        <v>44909</v>
       </c>
       <c r="L5" s="10">
         <f t="shared" ca="1" si="0"/>
-        <v>44896</v>
+        <v>44910</v>
       </c>
       <c r="M5" s="10">
         <f t="shared" ca="1" si="0"/>
-        <v>44897</v>
+        <v>44911</v>
       </c>
       <c r="N5" s="10">
         <f t="shared" ca="1" si="0"/>
-        <v>44898</v>
+        <v>44912</v>
       </c>
       <c r="O5" s="12">
         <f t="shared" ca="1" si="0"/>
-        <v>44899</v>
+        <v>44913</v>
       </c>
       <c r="P5" s="11">
         <f ca="1">O5+1</f>
-        <v>44900</v>
+        <v>44914</v>
       </c>
       <c r="Q5" s="10">
         <f ca="1">P5+1</f>
-        <v>44901</v>
+        <v>44915</v>
       </c>
       <c r="R5" s="10">
         <f t="shared" ca="1" si="0"/>
-        <v>44902</v>
+        <v>44916</v>
       </c>
       <c r="S5" s="10">
         <f t="shared" ca="1" si="0"/>
-        <v>44903</v>
+        <v>44917</v>
       </c>
       <c r="T5" s="10">
         <f t="shared" ca="1" si="0"/>
-        <v>44904</v>
+        <v>44918</v>
       </c>
       <c r="U5" s="10">
         <f t="shared" ca="1" si="0"/>
-        <v>44905</v>
+        <v>44919</v>
       </c>
       <c r="V5" s="12">
         <f t="shared" ca="1" si="0"/>
-        <v>44906</v>
+        <v>44920</v>
       </c>
       <c r="W5" s="11">
         <f ca="1">V5+1</f>
-        <v>44907</v>
+        <v>44921</v>
       </c>
       <c r="X5" s="10">
         <f ca="1">W5+1</f>
-        <v>44908</v>
+        <v>44922</v>
       </c>
       <c r="Y5" s="10">
         <f t="shared" ca="1" si="0"/>
-        <v>44909</v>
+        <v>44923</v>
       </c>
       <c r="Z5" s="10">
         <f t="shared" ca="1" si="0"/>
-        <v>44910</v>
+        <v>44924</v>
       </c>
       <c r="AA5" s="10">
         <f t="shared" ca="1" si="0"/>
-        <v>44911</v>
+        <v>44925</v>
       </c>
       <c r="AB5" s="10">
         <f t="shared" ca="1" si="0"/>
-        <v>44912</v>
+        <v>44926</v>
       </c>
       <c r="AC5" s="12">
         <f t="shared" ca="1" si="0"/>
-        <v>44913</v>
+        <v>44927</v>
       </c>
       <c r="AD5" s="11">
         <f ca="1">AC5+1</f>
-        <v>44914</v>
+        <v>44928</v>
       </c>
       <c r="AE5" s="10">
         <f ca="1">AD5+1</f>
-        <v>44915</v>
+        <v>44929</v>
       </c>
       <c r="AF5" s="10">
         <f t="shared" ca="1" si="0"/>
-        <v>44916</v>
+        <v>44930</v>
       </c>
       <c r="AG5" s="10">
         <f t="shared" ca="1" si="0"/>
-        <v>44917</v>
+        <v>44931</v>
       </c>
       <c r="AH5" s="10">
         <f t="shared" ca="1" si="0"/>
-        <v>44918</v>
+        <v>44932</v>
       </c>
       <c r="AI5" s="10">
         <f t="shared" ca="1" si="0"/>
-        <v>44919</v>
+        <v>44933</v>
       </c>
       <c r="AJ5" s="12">
         <f t="shared" ca="1" si="0"/>
-        <v>44920</v>
+        <v>44934</v>
       </c>
       <c r="AK5" s="11">
         <f ca="1">AJ5+1</f>
-        <v>44921</v>
+        <v>44935</v>
       </c>
       <c r="AL5" s="10">
         <f ca="1">AK5+1</f>
-        <v>44922</v>
+        <v>44936</v>
       </c>
       <c r="AM5" s="10">
         <f t="shared" ca="1" si="0"/>
-        <v>44923</v>
+        <v>44937</v>
       </c>
       <c r="AN5" s="10">
         <f t="shared" ca="1" si="0"/>
-        <v>44924</v>
+        <v>44938</v>
       </c>
       <c r="AO5" s="10">
         <f t="shared" ca="1" si="0"/>
-        <v>44925</v>
+        <v>44939</v>
       </c>
       <c r="AP5" s="10">
         <f t="shared" ca="1" si="0"/>
-        <v>44926</v>
+        <v>44940</v>
       </c>
       <c r="AQ5" s="12">
         <f t="shared" ca="1" si="0"/>
-        <v>44927</v>
+        <v>44941</v>
       </c>
       <c r="AR5" s="11">
         <f ca="1">AQ5+1</f>
-        <v>44928</v>
+        <v>44942</v>
       </c>
       <c r="AS5" s="10">
         <f ca="1">AR5+1</f>
-        <v>44929</v>
+        <v>44943</v>
       </c>
       <c r="AT5" s="10">
         <f t="shared" ca="1" si="0"/>
-        <v>44930</v>
+        <v>44944</v>
       </c>
       <c r="AU5" s="10">
         <f t="shared" ca="1" si="0"/>
-        <v>44931</v>
+        <v>44945</v>
       </c>
       <c r="AV5" s="10">
         <f t="shared" ca="1" si="0"/>
-        <v>44932</v>
+        <v>44946</v>
       </c>
       <c r="AW5" s="10">
         <f t="shared" ca="1" si="0"/>
-        <v>44933</v>
+        <v>44947</v>
       </c>
       <c r="AX5" s="12">
         <f t="shared" ca="1" si="0"/>
-        <v>44934</v>
+        <v>44948</v>
       </c>
       <c r="AY5" s="11">
         <f ca="1">AX5+1</f>
-        <v>44935</v>
+        <v>44949</v>
       </c>
       <c r="AZ5" s="10">
         <f ca="1">AY5+1</f>
-        <v>44936</v>
+        <v>44950</v>
       </c>
       <c r="BA5" s="10">
         <f t="shared" ref="BA5:BE5" ca="1" si="1">AZ5+1</f>
-        <v>44937</v>
+        <v>44951</v>
       </c>
       <c r="BB5" s="10">
         <f t="shared" ca="1" si="1"/>
-        <v>44938</v>
+        <v>44952</v>
       </c>
       <c r="BC5" s="10">
         <f t="shared" ca="1" si="1"/>
-        <v>44939</v>
+        <v>44953</v>
       </c>
       <c r="BD5" s="10">
         <f t="shared" ca="1" si="1"/>
-        <v>44940</v>
+        <v>44954</v>
       </c>
       <c r="BE5" s="12">
         <f t="shared" ca="1" si="1"/>
-        <v>44941</v>
+        <v>44955</v>
       </c>
       <c r="BF5" s="11">
         <f ca="1">BE5+1</f>
-        <v>44942</v>
+        <v>44956</v>
       </c>
       <c r="BG5" s="10">
         <f ca="1">BF5+1</f>
-        <v>44943</v>
+        <v>44957</v>
       </c>
       <c r="BH5" s="10">
         <f t="shared" ref="BH5:BL5" ca="1" si="2">BG5+1</f>
-        <v>44944</v>
+        <v>44958</v>
       </c>
       <c r="BI5" s="10">
         <f t="shared" ca="1" si="2"/>
-        <v>44945</v>
+        <v>44959</v>
       </c>
       <c r="BJ5" s="10">
         <f t="shared" ca="1" si="2"/>
-        <v>44946</v>
+        <v>44960</v>
       </c>
       <c r="BK5" s="10">
         <f t="shared" ca="1" si="2"/>
-        <v>44947</v>
+        <v>44961</v>
       </c>
       <c r="BL5" s="12">
         <f t="shared" ca="1" si="2"/>
-        <v>44948</v>
+        <v>44962</v>
       </c>
     </row>
     <row r="6" spans="1:64" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
@@ -2199,7 +2202,7 @@
         <v>33</v>
       </c>
       <c r="B8" s="18" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="C8" s="68"/>
       <c r="D8" s="19"/>
@@ -2276,16 +2279,16 @@
         <v>34</v>
       </c>
       <c r="B9" s="80" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="C9" s="69" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="D9" s="22">
         <v>0.05</v>
       </c>
       <c r="E9" s="63" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="F9" s="63"/>
       <c r="G9" s="17"/>
@@ -2355,7 +2358,7 @@
         <v>35</v>
       </c>
       <c r="B10" s="23" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="C10" s="70"/>
       <c r="D10" s="24"/>
@@ -2426,10 +2429,10 @@
     <row r="11" spans="1:64" s="3" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A11" s="59"/>
       <c r="B11" s="81" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="C11" s="82" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="D11" s="27">
         <v>0.2</v>
@@ -2505,10 +2508,10 @@
     <row r="12" spans="1:64" s="3" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A12" s="58"/>
       <c r="B12" s="81" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="C12" s="82" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="D12" s="27">
         <v>0.4</v>
@@ -2586,7 +2589,7 @@
         <v>25</v>
       </c>
       <c r="B13" s="28" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="C13" s="71"/>
       <c r="D13" s="29"/>
@@ -2657,10 +2660,10 @@
     <row r="14" spans="1:64" s="3" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A14" s="58"/>
       <c r="B14" s="83" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="C14" s="72" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="D14" s="32">
         <v>0.6</v>
@@ -2809,7 +2812,7 @@
     <row r="16" spans="1:64" s="3" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A16" s="58"/>
       <c r="B16" s="84" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="C16" s="74"/>
       <c r="D16" s="37">
@@ -2886,10 +2889,10 @@
     <row r="17" spans="1:64" s="3" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A17" s="58"/>
       <c r="B17" s="84" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="C17" s="74" t="s">
-        <v>38</v>
+        <v>53</v>
       </c>
       <c r="D17" s="37">
         <v>1</v>
@@ -2908,7 +2911,9 @@
       </c>
       <c r="I17" s="44"/>
       <c r="J17" s="44"/>
-      <c r="K17" s="44"/>
+      <c r="K17" s="44" t="s">
+        <v>54</v>
+      </c>
       <c r="L17" s="44"/>
       <c r="M17" s="44"/>
       <c r="N17" s="44"/>
@@ -3119,11 +3124,6 @@
     </row>
   </sheetData>
   <mergeCells count="12">
-    <mergeCell ref="C3:D3"/>
-    <mergeCell ref="C4:D4"/>
-    <mergeCell ref="B5:G5"/>
-    <mergeCell ref="AK4:AQ4"/>
-    <mergeCell ref="AR4:AX4"/>
     <mergeCell ref="AY4:BE4"/>
     <mergeCell ref="BF4:BL4"/>
     <mergeCell ref="E3:F3"/>
@@ -3131,6 +3131,11 @@
     <mergeCell ref="P4:V4"/>
     <mergeCell ref="W4:AC4"/>
     <mergeCell ref="AD4:AJ4"/>
+    <mergeCell ref="C3:D3"/>
+    <mergeCell ref="C4:D4"/>
+    <mergeCell ref="B5:G5"/>
+    <mergeCell ref="AK4:AQ4"/>
+    <mergeCell ref="AR4:AX4"/>
   </mergeCells>
   <conditionalFormatting sqref="D7:D19">
     <cfRule type="dataBar" priority="18">

</xml_diff>